<commit_message>
Revert "mise à jour fichier excel"
This reverts commit b15725905d365d5053e80efaab21a910409817fe.
</commit_message>
<xml_diff>
--- a/uploads/Compliance relating to Construction and Operation of expansion capacity Exploitation phase .xlsx
+++ b/uploads/Compliance relating to Construction and Operation of expansion capacity Exploitation phase .xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="12240" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+  <si>
+    <t>Due date for action</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Input (information and documents required for compliance)</t>
+  </si>
+  <si>
+    <t>Output (deliverable resulting from compliance)</t>
+  </si>
+  <si>
+    <t>Risk/sanction</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Cam Iron</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
   <si>
     <t>Monitoring Items / Categories</t>
   </si>
@@ -68,31 +92,7 @@
     <t>Person in charge</t>
   </si>
   <si>
-    <t>Due date for action</t>
-  </si>
-  <si>
     <t>State authority accountable for compliance</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Input (information and documents required for compliance)</t>
-  </si>
-  <si>
-    <t>Output (deliverable resulting from compliance)</t>
-  </si>
-  <si>
-    <t>Risk/sanction</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Cam Iron</t>
-  </si>
-  <si>
-    <t>State</t>
   </si>
   <si>
     <t xml:space="preserve">Construction and Operation of the Expansion Capacity </t>
@@ -150,7 +150,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,8 +159,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -178,21 +187,46 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -201,68 +235,173 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
+      <top style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -271,54 +410,190 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1085850</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 41"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1" noTextEdit="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="15592425" cy="1733550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1085850</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 41"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1" noTextEdit="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="15592425" cy="1733550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -606,193 +881,397 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:M9"/>
+  <dimension ref="A1:P109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="4" width="33" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:13">
-      <c r="A4" s="6" t="s">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="33" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" s="4" customFormat="1" ht="18" customHeight="1">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" customFormat="1" ht="33" customHeight="1" thickBot="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:16" s="10" customFormat="1" ht="44.25" customHeight="1" thickBot="1">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="I4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="J4" s="8"/>
+      <c r="K4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="L4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="M4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="6" t="s">
+    </row>
+    <row r="5" spans="1:16" customFormat="1" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="J5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="14"/>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="12"/>
+    <row r="6" spans="1:16" customFormat="1" ht="125.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21"/>
     </row>
-    <row r="6" spans="1:13" ht="409.5">
-      <c r="A6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
+    <row r="7" spans="1:16" customFormat="1" ht="99" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="23"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="21"/>
+    </row>
+    <row r="8" spans="1:16" customFormat="1" ht="77.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A8" s="15"/>
+      <c r="B8" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="3"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="21"/>
     </row>
-    <row r="7" spans="1:13" ht="409.5">
-      <c r="A7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="3"/>
+    <row r="9" spans="1:16" customFormat="1" ht="86.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="28"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="29"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="21"/>
     </row>
-    <row r="8" spans="1:13" ht="409.5">
-      <c r="A8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="3"/>
+    <row r="10" spans="1:16" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
     </row>
-    <row r="9" spans="1:13" ht="409.5">
-      <c r="A9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="3"/>
+    <row r="11" spans="1:16" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="33"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
+    <row r="12" spans="1:16" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="33"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="33"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="33"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" customFormat="1" ht="20.100000000000001" customHeight="1"/>
+    <row r="16" spans="1:16" customFormat="1" ht="20.100000000000001" customHeight="1"/>
+    <row r="17" customFormat="1"/>
+    <row r="18" customFormat="1"/>
+    <row r="19" customFormat="1"/>
+    <row r="20" customFormat="1" ht="46.5" customHeight="1"/>
+    <row r="21" customFormat="1"/>
+    <row r="22" customFormat="1"/>
+    <row r="23" customFormat="1"/>
+    <row r="24" customFormat="1" ht="76.5" customHeight="1"/>
+    <row r="25" customFormat="1"/>
+    <row r="26" customFormat="1"/>
+    <row r="27" customFormat="1"/>
+    <row r="28" customFormat="1" ht="16.5" customHeight="1"/>
+    <row r="29" customFormat="1"/>
+    <row r="30" customFormat="1" ht="31.5" customHeight="1"/>
+    <row r="31" customFormat="1"/>
+    <row r="32" customFormat="1"/>
+    <row r="33" customFormat="1"/>
+    <row r="34" customFormat="1"/>
+    <row r="35" customFormat="1" ht="46.5" customHeight="1"/>
+    <row r="36" customFormat="1"/>
+    <row r="37" customFormat="1"/>
+    <row r="38" customFormat="1" ht="31.5" customHeight="1"/>
+    <row r="39" customFormat="1"/>
+    <row r="40" customFormat="1"/>
+    <row r="41" customFormat="1"/>
+    <row r="42" customFormat="1"/>
+    <row r="43" customFormat="1" ht="46.5" customHeight="1"/>
+    <row r="44" customFormat="1"/>
+    <row r="45" customFormat="1" ht="61.5" customHeight="1"/>
+    <row r="46" customFormat="1"/>
+    <row r="47" customFormat="1"/>
+    <row r="48" customFormat="1"/>
+    <row r="49" customFormat="1" ht="16.5" customHeight="1"/>
+    <row r="50" customFormat="1"/>
+    <row r="51" customFormat="1" ht="46.5" customHeight="1"/>
+    <row r="52" customFormat="1"/>
+    <row r="53" customFormat="1"/>
+    <row r="54" customFormat="1" ht="16.5" customHeight="1"/>
+    <row r="55" customFormat="1"/>
+    <row r="56" customFormat="1"/>
+    <row r="57" customFormat="1"/>
+    <row r="58" customFormat="1" ht="31.5" customHeight="1"/>
+    <row r="59" customFormat="1"/>
+    <row r="60" customFormat="1"/>
+    <row r="61" customFormat="1"/>
+    <row r="62" customFormat="1" ht="31.5" customHeight="1"/>
+    <row r="63" customFormat="1"/>
+    <row r="64" customFormat="1"/>
+    <row r="65" customFormat="1"/>
+    <row r="66" customFormat="1" ht="31.5" customHeight="1"/>
+    <row r="67" customFormat="1"/>
+    <row r="68" customFormat="1"/>
+    <row r="69" customFormat="1"/>
+    <row r="70" customFormat="1" ht="31.5" customHeight="1"/>
+    <row r="71" customFormat="1"/>
+    <row r="72" customFormat="1"/>
+    <row r="73" customFormat="1"/>
+    <row r="74" customFormat="1" ht="16.5" customHeight="1"/>
+    <row r="75" customFormat="1"/>
+    <row r="76" customFormat="1"/>
+    <row r="77" customFormat="1"/>
+    <row r="78" customFormat="1"/>
+    <row r="79" customFormat="1" ht="16.5" customHeight="1"/>
+    <row r="80" customFormat="1"/>
+    <row r="81" customFormat="1"/>
+    <row r="82" customFormat="1"/>
+    <row r="83" customFormat="1"/>
+    <row r="84" customFormat="1" ht="31.5" customHeight="1"/>
+    <row r="85" customFormat="1"/>
+    <row r="86" customFormat="1"/>
+    <row r="87" customFormat="1"/>
+    <row r="88" customFormat="1"/>
+    <row r="89" customFormat="1"/>
+    <row r="90" customFormat="1" ht="31.5" customHeight="1"/>
+    <row r="91" customFormat="1"/>
+    <row r="92" customFormat="1" ht="31.5" customHeight="1"/>
+    <row r="93" customFormat="1"/>
+    <row r="94" customFormat="1" ht="31.5" customHeight="1"/>
+    <row r="95" customFormat="1"/>
+    <row r="96" customFormat="1" ht="16.5" customHeight="1"/>
+    <row r="97" customFormat="1" ht="20.100000000000001" customHeight="1"/>
+    <row r="98" customFormat="1" ht="20.100000000000001" customHeight="1"/>
+    <row r="99" customFormat="1" ht="17.25" customHeight="1"/>
+    <row r="100" customFormat="1" ht="20.100000000000001" customHeight="1"/>
+    <row r="101" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="102" customFormat="1" ht="18.75" customHeight="1"/>
+    <row r="103" customFormat="1" ht="36" customHeight="1"/>
+    <row r="104" customFormat="1" ht="28.5" customHeight="1"/>
+    <row r="105" customFormat="1" ht="25.5" customHeight="1"/>
+    <row r="106" customFormat="1" ht="27.75" customHeight="1"/>
+    <row r="107" customFormat="1" ht="18" customHeight="1"/>
+    <row r="108" customFormat="1" ht="22.5" customHeight="1"/>
+    <row r="109" customFormat="1" ht="76.5" customHeight="1"/>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:J4"/>
+  <mergeCells count="14">
+    <mergeCell ref="L6:L9"/>
+    <mergeCell ref="A6:A9"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="M4:M5"/>
@@ -802,9 +1281,14 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>